<commit_message>
Added category / sub to valuations
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments.xlsx
+++ b/public/sample_uploads/portfolio_investments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A38DBDC-5438-41A0-AF41-27A46B808A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A39509-80A7-4CEC-B7D5-D2FE94497E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Quantity *</t>
   </si>
   <si>
-    <t>Investment Type *</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -51,34 +48,58 @@
     <t>Apple</t>
   </si>
   <si>
+    <t>Bought during dip</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>KLAC</t>
+  </si>
+  <si>
+    <t>SAAS Fund</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Folio No</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>CoInvest</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>Investment Domicile</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Unlisted</t>
+  </si>
+  <si>
     <t>Equity</t>
-  </si>
-  <si>
-    <t>Bought during dip</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>KLAC</t>
-  </si>
-  <si>
-    <t>SAAS Fund</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Folio No</t>
-  </si>
-  <si>
-    <t>Pool</t>
-  </si>
-  <si>
-    <t>CoInvest</t>
-  </si>
-  <si>
-    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -397,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J3" sqref="J3:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -408,12 +429,11 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -431,21 +451,33 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>43831</v>
@@ -457,21 +489,30 @@
         <v>20000</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>43831</v>
@@ -483,21 +524,30 @@
         <v>12000</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>43831</v>
@@ -509,21 +559,30 @@
         <v>-20000</v>
       </c>
       <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>43831</v>
@@ -535,21 +594,30 @@
         <v>10000</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>44197</v>
@@ -561,21 +629,30 @@
         <v>20000</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>44197</v>
@@ -587,24 +664,33 @@
         <v>12000</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>43831</v>
@@ -616,21 +702,30 @@
         <v>20000</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>43831</v>
@@ -642,13 +737,22 @@
         <v>-10000</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test for CF for portfolio investments
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments.xlsx
+++ b/public/sample_uploads/portfolio_investments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9081D28-B13B-43D3-9993-9E556DBEA688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B21DF95-E651-470C-A982-F61E927AE3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Portfolio Company Name *</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Investment Domicile *</t>
+  </si>
+  <si>
+    <t>Custom Field 1</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="O3" sqref="O3:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -461,7 +467,7 @@
     <col min="12" max="12" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -504,8 +510,11 @@
       <c r="N1" t="s">
         <v>28</v>
       </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -542,17 +551,18 @@
       <c r="N2" t="s">
         <v>17</v>
       </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="1">
         <v>43831</v>
       </c>
@@ -580,17 +590,18 @@
       <c r="N3" t="s">
         <v>17</v>
       </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="1">
         <v>43831</v>
       </c>
@@ -618,8 +629,11 @@
       <c r="N4" t="s">
         <v>17</v>
       </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -656,8 +670,11 @@
       <c r="N5" t="s">
         <v>17</v>
       </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -694,17 +711,18 @@
       <c r="N6" t="s">
         <v>17</v>
       </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="1">
         <v>44197</v>
       </c>
@@ -735,8 +753,11 @@
       <c r="N7" t="s">
         <v>17</v>
       </c>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -773,17 +794,18 @@
       <c r="N8" t="s">
         <v>17</v>
       </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1">
         <v>43831</v>
       </c>
@@ -810,6 +832,9 @@
       </c>
       <c r="N9" t="s">
         <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transaction and idempotency to PortfolioAttribution
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments.xlsx
+++ b/public/sample_uploads/portfolio_investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAD2ED8-E8B9-4895-83E0-9913867B9019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1326D5-33A3-4456-80FE-AA32E774F892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -482,6 +482,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="22.1328125" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.9296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.3984375" customWidth="1"/>
     <col min="1023" max="1023" width="9.1328125" customWidth="1"/>
   </cols>
@@ -573,7 +574,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>43831</v>
+        <v>44197</v>
       </c>
       <c r="D3">
         <v>1000000</v>
@@ -611,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="1">
-        <v>43831</v>
+        <v>44562</v>
       </c>
       <c r="D4">
         <v>2000000</v>
@@ -687,13 +688,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="1">
-        <v>44197</v>
+        <v>44927</v>
       </c>
       <c r="D6">
         <v>2000000</v>
       </c>
       <c r="E6">
-        <v>20000</v>
+        <v>-3000</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Fixed import of PI and Investment instrument uniqueness
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments.xlsx
+++ b/public/sample_uploads/portfolio_investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F2DF6B-0650-4423-805F-551A486ED6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CA039F-34E1-4021-9335-D3F623CBEBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,32 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Applicable if for CoInvest</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Fund</t>
   </si>
@@ -248,9 +223,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Folio No</t>
   </si>
   <si>
     <t>Instrument</t>
@@ -696,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMA9"/>
+  <dimension ref="A1:ALZ9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -709,20 +681,19 @@
     <col min="3" max="3" width="16.265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.3984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.19921875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="10.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.19921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.9296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="29.265625" style="1" customWidth="1"/>
-    <col min="15" max="1014" width="8.53125" style="1"/>
-    <col min="1015" max="1015" width="9.1328125" style="1" customWidth="1"/>
-    <col min="1016" max="1024" width="9.1328125" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.19921875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.9296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.265625" style="1" customWidth="1"/>
+    <col min="14" max="1013" width="8.53125" style="1"/>
+    <col min="1014" max="1014" width="9.1328125" style="1" customWidth="1"/>
+    <col min="1015" max="1023" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -733,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -745,25 +716,22 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="ALW1"/>
       <c r="ALX1"/>
       <c r="ALY1"/>
       <c r="ALZ1"/>
-      <c r="AMA1"/>
     </row>
-    <row r="2" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="3">
         <v>43831</v>
@@ -775,24 +743,24 @@
         <v>20000</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>44197</v>
@@ -804,24 +772,24 @@
         <v>12000</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>44562</v>
@@ -833,24 +801,24 @@
         <v>-20000</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:1014" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1015" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>43831</v>
@@ -862,24 +830,24 @@
         <v>10000</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="6" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>44927</v>
@@ -891,24 +859,24 @@
         <v>-3000</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="7" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>44228</v>
@@ -920,24 +888,24 @@
         <v>12000</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="8" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
         <v>43831</v>
@@ -949,24 +917,24 @@
         <v>20000</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="9" spans="1:1015" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1014" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
         <v>43831</v>
@@ -978,21 +946,21 @@
         <v>-10000</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1009" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1009" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Domestic,Overseas"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>